<commit_message>
sankey progress 1,2 axis
</commit_message>
<xml_diff>
--- a/output/excel-organize_final.xlsx
+++ b/output/excel-organize_final.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karanshakya/Desktop/mom-ag_services/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA952CE9-1CA4-BA49-9AFB-BCC0ABE6562D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556F641F-FD45-394A-A4B7-3AF7F9F5CADE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{D48A5087-0F85-9648-B34D-C644C0BC30EB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{D48A5087-0F85-9648-B34D-C644C0BC30EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Year" sheetId="6" r:id="rId1"/>
     <sheet name="Country" sheetId="5" r:id="rId2"/>
     <sheet name="Combined 5 Years" sheetId="7" r:id="rId3"/>
+    <sheet name="Institution - Country List" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6497" uniqueCount="4986">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6583" uniqueCount="5062">
   <si>
     <t>"conservation",</t>
   </si>
@@ -14993,6 +14994,257 @@
   </si>
   <si>
     <t>Combined Keywords (Author + Index)</t>
+  </si>
+  <si>
+    <t>(IFPRI)</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>Arabia</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Assam</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Emirates</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Faso</t>
+  </si>
+  <si>
+    <t>Federation</t>
+  </si>
+  <si>
+    <t>Fiji</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>India.</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>International</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Japan.</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Kingdom</t>
+  </si>
+  <si>
+    <t>Kong</t>
+  </si>
+  <si>
+    <t>Korea</t>
+  </si>
+  <si>
+    <t>Kyrgyzstan</t>
+  </si>
+  <si>
+    <t>Lanka</t>
+  </si>
+  <si>
+    <t>Laos</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Oman</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Republic</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>States</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+  </si>
+  <si>
+    <t>Tajikistan</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Zealand</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Country count of where where authors are from. Taken from the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Affiliation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> column.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -15095,7 +15347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -15113,14 +15365,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -15835,58 +16090,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C212A0F-4070-6245-96AE-2111416C428E}">
   <dimension ref="B1:O3228"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>4985</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
     </row>
     <row r="3" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>455</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>456</v>
       </c>
-      <c r="F3" s="9"/>
+      <c r="F3" s="11"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="I3" s="9"/>
+      <c r="I3" s="11"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="11" t="s">
         <v>458</v>
       </c>
-      <c r="L3" s="9"/>
+      <c r="L3" s="11"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="9" t="s">
+      <c r="N3" s="11" t="s">
         <v>459</v>
       </c>
-      <c r="O3" s="9"/>
+      <c r="O3" s="11"/>
     </row>
     <row r="4" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>477</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -15917,7 +16172,7 @@
       <c r="N4" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="O4" s="12" t="s">
+      <c r="O4" s="10" t="s">
         <v>450</v>
       </c>
     </row>
@@ -61137,13 +61392,974 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B1:O1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="N3:O3"/>
-    <mergeCell ref="B1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D27632-CDBC-F44A-9F52-5AD617144226}">
+  <dimension ref="B1:H87"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B1" s="13" t="s">
+        <v>5061</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D3" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>463</v>
+      </c>
+      <c r="E4">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>462</v>
+      </c>
+      <c r="E5">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5051</v>
+      </c>
+      <c r="E6">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>464</v>
+      </c>
+      <c r="E7">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5023</v>
+      </c>
+      <c r="E8">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>465</v>
+      </c>
+      <c r="E9">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4991</v>
+      </c>
+      <c r="E10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>460</v>
+      </c>
+      <c r="E11">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5011</v>
+      </c>
+      <c r="E12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5018</v>
+      </c>
+      <c r="E13">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4999</v>
+      </c>
+      <c r="E14">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5019</v>
+      </c>
+      <c r="E15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5009</v>
+      </c>
+      <c r="E16">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>471</v>
+      </c>
+      <c r="E17">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5035</v>
+      </c>
+      <c r="E18">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5056</v>
+      </c>
+      <c r="E19">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>461</v>
+      </c>
+      <c r="E20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5029</v>
+      </c>
+      <c r="E21">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>19</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5050</v>
+      </c>
+      <c r="E22">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5041</v>
+      </c>
+      <c r="E23">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>5022</v>
+      </c>
+      <c r="E24">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5053</v>
+      </c>
+      <c r="E25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <v>23</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5048</v>
+      </c>
+      <c r="E26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <v>24</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5052</v>
+      </c>
+      <c r="E27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <v>25</v>
+      </c>
+      <c r="D28" t="s">
+        <v>4997</v>
+      </c>
+      <c r="E28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <v>26</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5025</v>
+      </c>
+      <c r="E29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <v>27</v>
+      </c>
+      <c r="D30" t="s">
+        <v>5034</v>
+      </c>
+      <c r="E30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <v>28</v>
+      </c>
+      <c r="D31" t="s">
+        <v>5038</v>
+      </c>
+      <c r="E31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <v>29</v>
+      </c>
+      <c r="D32" t="s">
+        <v>5001</v>
+      </c>
+      <c r="E32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <v>30</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5014</v>
+      </c>
+      <c r="E33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <v>31</v>
+      </c>
+      <c r="D34" t="s">
+        <v>4994</v>
+      </c>
+      <c r="E34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <v>32</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5024</v>
+      </c>
+      <c r="E35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <v>33</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5030</v>
+      </c>
+      <c r="E36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <v>34</v>
+      </c>
+      <c r="D37" t="s">
+        <v>4987</v>
+      </c>
+      <c r="E37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C38">
+        <v>35</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5000</v>
+      </c>
+      <c r="E38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <v>36</v>
+      </c>
+      <c r="D39" t="s">
+        <v>5004</v>
+      </c>
+      <c r="E39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <v>37</v>
+      </c>
+      <c r="D40" t="s">
+        <v>5006</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <v>38</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5054</v>
+      </c>
+      <c r="E41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <v>39</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5008</v>
+      </c>
+      <c r="E42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <v>40</v>
+      </c>
+      <c r="D43" t="s">
+        <v>5010</v>
+      </c>
+      <c r="E43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C44">
+        <v>41</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5017</v>
+      </c>
+      <c r="E44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C45">
+        <v>42</v>
+      </c>
+      <c r="D45" t="s">
+        <v>5058</v>
+      </c>
+      <c r="E45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C46">
+        <v>43</v>
+      </c>
+      <c r="D46" t="s">
+        <v>4988</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C47">
+        <v>44</v>
+      </c>
+      <c r="D47" t="s">
+        <v>5027</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C48">
+        <v>45</v>
+      </c>
+      <c r="D48" t="s">
+        <v>5039</v>
+      </c>
+      <c r="E48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C49">
+        <v>46</v>
+      </c>
+      <c r="D49" t="s">
+        <v>5040</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C50">
+        <v>47</v>
+      </c>
+      <c r="D50" t="s">
+        <v>5059</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C51">
+        <v>48</v>
+      </c>
+      <c r="D51" t="s">
+        <v>5060</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C52">
+        <v>49</v>
+      </c>
+      <c r="D52" t="s">
+        <v>469</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C53">
+        <v>50</v>
+      </c>
+      <c r="D53" t="s">
+        <v>4989</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C54">
+        <v>51</v>
+      </c>
+      <c r="D54" t="s">
+        <v>4993</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C55">
+        <v>52</v>
+      </c>
+      <c r="D55" t="s">
+        <v>4998</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C56">
+        <v>53</v>
+      </c>
+      <c r="D56" t="s">
+        <v>5003</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C57">
+        <v>54</v>
+      </c>
+      <c r="D57" t="s">
+        <v>5026</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C58">
+        <v>55</v>
+      </c>
+      <c r="D58" t="s">
+        <v>5028</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C59">
+        <v>56</v>
+      </c>
+      <c r="D59" t="s">
+        <v>5042</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C60">
+        <v>57</v>
+      </c>
+      <c r="D60" t="s">
+        <v>5044</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C61">
+        <v>58</v>
+      </c>
+      <c r="D61" t="s">
+        <v>5047</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C62">
+        <v>59</v>
+      </c>
+      <c r="D62" t="s">
+        <v>5057</v>
+      </c>
+      <c r="E62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C63">
+        <v>60</v>
+      </c>
+      <c r="D63" t="s">
+        <v>4986</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C64">
+        <v>61</v>
+      </c>
+      <c r="D64">
+        <v>650205</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C65">
+        <v>62</v>
+      </c>
+      <c r="D65" t="s">
+        <v>4990</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C66">
+        <v>63</v>
+      </c>
+      <c r="D66" t="s">
+        <v>4992</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C67">
+        <v>64</v>
+      </c>
+      <c r="D67" t="s">
+        <v>4995</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C68">
+        <v>65</v>
+      </c>
+      <c r="D68" t="s">
+        <v>4996</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C69">
+        <v>66</v>
+      </c>
+      <c r="D69" t="s">
+        <v>5002</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C70">
+        <v>67</v>
+      </c>
+      <c r="D70" t="s">
+        <v>5005</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C71">
+        <v>68</v>
+      </c>
+      <c r="D71" t="s">
+        <v>5007</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C72">
+        <v>69</v>
+      </c>
+      <c r="D72" t="s">
+        <v>5012</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C73">
+        <v>70</v>
+      </c>
+      <c r="D73" t="s">
+        <v>5013</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C74">
+        <v>71</v>
+      </c>
+      <c r="D74" t="s">
+        <v>5015</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C75">
+        <v>72</v>
+      </c>
+      <c r="D75" t="s">
+        <v>5016</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C76">
+        <v>73</v>
+      </c>
+      <c r="D76" t="s">
+        <v>5020</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C77">
+        <v>74</v>
+      </c>
+      <c r="D77" t="s">
+        <v>5021</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C78">
+        <v>75</v>
+      </c>
+      <c r="D78" t="s">
+        <v>5031</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C79">
+        <v>76</v>
+      </c>
+      <c r="D79" t="s">
+        <v>5032</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C80">
+        <v>77</v>
+      </c>
+      <c r="D80" t="s">
+        <v>5033</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C81">
+        <v>78</v>
+      </c>
+      <c r="D81" t="s">
+        <v>5036</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C82">
+        <v>79</v>
+      </c>
+      <c r="D82" t="s">
+        <v>5037</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C83">
+        <v>80</v>
+      </c>
+      <c r="D83" t="s">
+        <v>5043</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C84">
+        <v>81</v>
+      </c>
+      <c r="D84" t="s">
+        <v>5045</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C85">
+        <v>82</v>
+      </c>
+      <c r="D85" t="s">
+        <v>5046</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C86">
+        <v>83</v>
+      </c>
+      <c r="D86" t="s">
+        <v>5049</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C87">
+        <v>84</v>
+      </c>
+      <c r="D87" t="s">
+        <v>5055</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C4:E87">
+    <sortCondition descending="1" ref="E4:E87"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
figure edits - code checks - trouble shooting
</commit_message>
<xml_diff>
--- a/output/excel-organize_final.xlsx
+++ b/output/excel-organize_final.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karanshakya/Desktop/mom-ag_services/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556F641F-FD45-394A-A4B7-3AF7F9F5CADE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A61538-8727-5A40-B3A6-950AD424F3EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{D48A5087-0F85-9648-B34D-C644C0BC30EB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{D48A5087-0F85-9648-B34D-C644C0BC30EB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Year" sheetId="6" r:id="rId1"/>
-    <sheet name="Country" sheetId="5" r:id="rId2"/>
+    <sheet name="Year Summary" sheetId="6" r:id="rId1"/>
+    <sheet name="Country Summary" sheetId="5" r:id="rId2"/>
     <sheet name="Combined 5 Years" sheetId="7" r:id="rId3"/>
-    <sheet name="Institution - Country List" sheetId="8" r:id="rId4"/>
+    <sheet name="Institution - Collaboration" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -15367,14 +15367,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -15391,6 +15391,104 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E58F946-5AF3-5F44-B9C3-A6A22A805F1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="444500"/>
+          <a:ext cx="5448300" cy="3632200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>741916</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAD03529-B1B1-954A-A326-AC35D37D107F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6654800" y="1155700"/>
+          <a:ext cx="8120616" cy="5372100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15693,7 +15791,7 @@
   <dimension ref="C2:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15933,7 +16031,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F55496-8323-2E4F-B6FF-EEBDAF054BB5}">
   <dimension ref="C2:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16083,6 +16183,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -16091,7 +16192,7 @@
   <dimension ref="B1:O3228"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:O22"/>
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16115,30 +16216,30 @@
       <c r="O1" s="12"/>
     </row>
     <row r="3" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="13" t="s">
         <v>455</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="13"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="13" t="s">
         <v>456</v>
       </c>
-      <c r="F3" s="11"/>
+      <c r="F3" s="13"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="13" t="s">
         <v>457</v>
       </c>
-      <c r="I3" s="11"/>
+      <c r="I3" s="13"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="L3" s="11"/>
+      <c r="L3" s="13"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="11" t="s">
+      <c r="N3" s="13" t="s">
         <v>459</v>
       </c>
-      <c r="O3" s="11"/>
+      <c r="O3" s="13"/>
     </row>
     <row r="4" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
@@ -61407,22 +61508,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D27632-CDBC-F44A-9F52-5AD617144226}">
   <dimension ref="B1:H87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>5061</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D3" s="3" t="s">
@@ -62361,5 +62462,6 @@
     <sortCondition descending="1" ref="E4:E87"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>